<commit_message>
Filtering data for specific values
</commit_message>
<xml_diff>
--- a/Data/Ghost crab burrow architecture.xlsx
+++ b/Data/Ghost crab burrow architecture.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9090739D-3741-4A68-A678-22B08C4607E3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4D6CFC-FEE9-4ECE-8B04-294B2C05143C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>